<commit_message>
minor changes in model field (renaming)
</commit_message>
<xml_diff>
--- a/backend/templates/StudentTemplate.xlsx
+++ b/backend/templates/StudentTemplate.xlsx
@@ -608,7 +608,7 @@
       <c r="F4" s="2" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="20">
+  <dataValidations count="21">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Male, Female, Others"</formula1>
     </dataValidation>
@@ -667,8 +667,11 @@
     <dataValidation sqref="I2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Option" error="This is not a valid option" type="list">
       <formula1>=InstructorList!$A$1:$A$53</formula1>
     </dataValidation>
+    <dataValidation sqref="I2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Option" error="This is not a valid option" type="list">
+      <formula1>=InstructorList!$A$1:$A$53</formula1>
+    </dataValidation>
     <dataValidation sqref="I2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Option" error="This is not a valid option" type="list">
-      <formula1>=InstructorList!$A$1:$A$53</formula1>
+      <formula1>=InstructorList!$A$1:$A$49</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -695,12 +698,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Anne Lopez</t>
+          <t>Amy Collins</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Christine559902@iiitd.ac.in</t>
+          <t>Sarah758717@iiitd.ac.in</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -712,576 +715,576 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>April Townsend</t>
+          <t>Angela Brown</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Michael140088@iiitd.ac.in</t>
+          <t>Alicia660431@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Brenda Yu</t>
+          <t>Anthony Hill</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hudson986478@iiitd.ac.in</t>
+          <t>Chloe189394@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Brian Martin</t>
+          <t>Barbara Ramirez</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Angela346858@iiitd.ac.in</t>
+          <t>Richard170293@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Brianna Lowe</t>
+          <t>Brian Ferguson</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chung715134@iiitd.ac.in</t>
+          <t>Jennings507360@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Christine Jones MD</t>
+          <t>Christine Esparza</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Collins121453@iiitd.ac.in</t>
+          <t>Fox154013@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Curtis Myers</t>
+          <t>Christopher Lowe</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cameron67453@iiitd.ac.in</t>
+          <t>Katelyn13372@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Daniel Adams</t>
+          <t>Cynthia Santiago</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Kaufman623654@iiitd.ac.in</t>
+          <t>Fernando672775@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>David Hernandez</t>
+          <t>Daniel Cole</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Austin166373@iiitd.ac.in</t>
+          <t>Bowers38862@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>David Preston</t>
+          <t>David Ramirez</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Melissa222506@iiitd.ac.in</t>
+          <t>Brown853382@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Debbie Howard</t>
+          <t>Dawn Green</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Garrett70426@iiitd.ac.in</t>
+          <t>Shannon490804@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Deborah Lester</t>
+          <t>Dawn Kelly</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Salazar784908@iiitd.ac.in</t>
+          <t>Elizabeth335384@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Derek Jones</t>
+          <t>Derrick Mann</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jessica441482@iiitd.ac.in</t>
+          <t>Erin371713@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Elaine Coffey</t>
+          <t>Dr. Tyler Lee Jr.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Williams70090@iiitd.ac.in</t>
+          <t>Kyle105952@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Erica Evans</t>
+          <t>Elizabeth Graham</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Alvarado267744@iiitd.ac.in</t>
+          <t>Baker893109@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Holly Sanders</t>
+          <t>Erin Hess</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Laurie142405@iiitd.ac.in</t>
+          <t>Moreno247722@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>James Rose</t>
+          <t>Gregory Ward</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Carly936829@iiitd.ac.in</t>
+          <t>Edwards592751@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jeffrey Velasquez</t>
+          <t>Heather Knapp</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Morgan554523@iiitd.ac.in</t>
+          <t>Morales187759@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jenna Farmer</t>
+          <t>Hunter Rhodes</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bright542835@iiitd.ac.in</t>
+          <t>Wagner715502@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jenna Wilson</t>
+          <t>Jeffrey Wolf DVM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>John676620@iiitd.ac.in</t>
+          <t>Davis954537@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jennifer Williams 2</t>
+          <t>Jeremy Jones Jr.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>West8865990@iiitd.ac.in</t>
+          <t>Dawn511100@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jerry Thompson</t>
+          <t>Joel Medina</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Frank579887@iiitd.ac.in</t>
+          <t>Frost896290@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Jonathan Hughes</t>
+          <t>Joseph Hughes</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Robin855679@iiitd.ac.in</t>
+          <t>Mackenzie507047@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Joshua Hughes</t>
+          <t>Joseph Tucker</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Carol293243@iiitd.ac.in</t>
+          <t>Cody602101@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Katherine Huffman</t>
+          <t>Joshua Smith</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Maynard913684@iiitd.ac.in</t>
+          <t>Myers657868@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Kelly Melendez</t>
+          <t>Julie Frey</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Chavez271173@iiitd.ac.in</t>
+          <t>Curtis759699@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Kevin Walker</t>
+          <t>Karen Johnson</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Emma136076@iiitd.ac.in</t>
+          <t>Galvan651884@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Laura Calhoun</t>
+          <t>Kathryn Dodson</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Massey874466@iiitd.ac.in</t>
+          <t>Nelson333547@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lisa Fleming</t>
+          <t>Katrina Morris</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Molly343344@iiitd.ac.in</t>
+          <t>Tapia875113@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Marisa Rodriguez</t>
+          <t>Kayla Sanders</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>King188862@iiitd.ac.in</t>
+          <t>Nicole76334@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mark Myers</t>
+          <t>Kevin Thomas</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Danielle702158@iiitd.ac.in</t>
+          <t>Angela516762@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Michael Munoz</t>
+          <t>Kyle Campos</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hall802103@iiitd.ac.in</t>
+          <t>Evans535740@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Morgan Stanley</t>
+          <t>Laura Velazquez</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Morales282564@iiitd.ac.in</t>
+          <t>Haynes397330@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mr. Jeffrey Baker</t>
+          <t>Lauren Griffith</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Anderson125566@iiitd.ac.in</t>
+          <t>Ronald686785@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mrs. Tara Morales MD</t>
+          <t>Linda Davis</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Patricia94254@iiitd.ac.in</t>
+          <t>Tiffany178877@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Nicholas Baxter</t>
+          <t>Mary Carter</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Taylor984862@iiitd.ac.in</t>
+          <t>Gonzalez239104@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Noah Farmer</t>
+          <t>Matthew Garcia</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Travis170197@iiitd.ac.in</t>
+          <t>Jessica496901@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Olivia Hall</t>
+          <t>Melissa Little</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Edward834545@iiitd.ac.in</t>
+          <t>Hall656983@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Prof 1</t>
+          <t>Michael Cunningham</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>prof1@iiitd.ac.in</t>
+          <t>Mitchell274929@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Prof 5</t>
+          <t>Michele Stewart</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>prof3@iiitd.ac.in</t>
+          <t>Paul165761@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Robert Gonzalez</t>
+          <t>Nathan Hudson</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Nelson72089@iiitd.ac.in</t>
+          <t>Day871043@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ryan Harris</t>
+          <t>Nicole Anderson</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Julie339932@iiitd.ac.in</t>
+          <t>Solomon359603@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Samuel Snyder</t>
+          <t>Prof 1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Whitehead791749@iiitd.ac.in</t>
+          <t>prof1@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sarah Thompson</t>
+          <t>Randall Villegas PhD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Diaz332222@iiitd.ac.in</t>
+          <t>Michelle408719@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Shannon Park</t>
+          <t>Robert White</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Justin973091@iiitd.ac.in</t>
+          <t>Brown17101@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Stanley Ochoa</t>
+          <t>Ryan Ramirez</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Nixon61903@iiitd.ac.in</t>
+          <t>Nicole236280@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Stephanie Smith</t>
+          <t>Steven Reyes</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Michael221872@iiitd.ac.in</t>
+          <t>Elizabeth926807@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Super Advisor</t>
+          <t>Tracy Freeman</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>superinstr@iiitd.ac.in</t>
+          <t>Bennett384108@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Tanya Mccarthy</t>
+          <t>Victor Harrison</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Rice292805@iiitd.ac.in</t>
+          <t>Jodi306564@iiitd.ac.in</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed: Advisor drop down list limited to 50 options in StudentTemplate Excel file
</commit_message>
<xml_diff>
--- a/backend/templates/StudentTemplate.xlsx
+++ b/backend/templates/StudentTemplate.xlsx
@@ -9,7 +9,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="InstructorList" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="InstructorNames">OFFSET(InstructorList!$A$1, 0, 0, COUNTA(InstructorList!$A:$A), 1)</definedName>
+  </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -19,7 +21,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,12 +35,6 @@
       <color theme="10"/>
       <sz val="11"/>
       <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -473,8 +469,8 @@
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S2" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" customHeight="1"/>
@@ -635,7 +631,7 @@
       <c r="F4" s="2" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="18">
+  <dataValidations count="19">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Male, Female, Others"</formula1>
     </dataValidation>
@@ -672,7 +668,7 @@
     <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Institute, Sponsored, Others"</formula1>
     </dataValidation>
-    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid input value" error="Input value should be between 0 and 99,99,99,999" type="decimal">
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid input value" error="Input value should be between 0 and 99,99,99,999" prompt="Default value is 20000 (if left empty)" type="decimal">
       <formula1>0</formula1>
       <formula2>999999999</formula2>
     </dataValidation>
@@ -685,11 +681,14 @@
     <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>2000</formula1>
     </dataValidation>
-    <dataValidation sqref="W2:X1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Input" error="Negative values not allowed" type="whole" operator="greaterThanOrEqual">
+    <dataValidation sqref="X2:X1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Input" error="Negative values not allowed" prompt="Default value is 4 (if left empty)" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation sqref="I2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Option" error="This is not a valid option" type="list">
-      <formula1>=InstructorList!$A$1:$A$50</formula1>
+    <dataValidation sqref="I2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Option" error="This is not a valid option" type="list">
+      <formula1>InstructorNames</formula1>
+    </dataValidation>
+    <dataValidation sqref="W2:W1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Input" error="Negative values not allowed" prompt="Default value is 60 (if left empty)" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -705,7 +704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,12 +715,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Alyssa Daugherty</t>
+          <t>Amy Conner</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Smith579513@iiitd.ac.in</t>
+          <t>Lynch109526@iiitd.ac.in</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -733,612 +732,648 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Amber Mann</t>
+          <t>Angel Cummings</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gray399786@iiitd.ac.in</t>
+          <t>Morris703534@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bradley Harris</t>
+          <t>Ashley Rodriguez</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mark583733@iiitd.ac.in</t>
+          <t>Michael483861@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Charles Long</t>
+          <t>Barbara Diaz</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Diane35794@iiitd.ac.in</t>
+          <t>Anita815630@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Charlotte Brown</t>
+          <t>Brett Jennings</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mclaughlin64751@iiitd.ac.in</t>
+          <t>Natalie195614@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Christina Ferrell</t>
+          <t>Brian Palmer</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Roberts235080@iiitd.ac.in</t>
+          <t>Haley631732@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cody Stevens</t>
+          <t>Brian Torres</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Barbara515971@iiitd.ac.in</t>
+          <t>Austin155422@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cynthia Moses</t>
+          <t>Casey Robinson</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Aguirre583317@iiitd.ac.in</t>
+          <t>Rogers164109@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Eileen Sims</t>
+          <t>Claire Delgado</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Thomas63431@iiitd.ac.in</t>
+          <t>Kyle493638@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Elizabeth Rojas</t>
+          <t>Courtney Webb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Robin103502@iiitd.ac.in</t>
+          <t>Holly726051@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>George Coleman</t>
+          <t>Crystal Allen</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>James52012@iiitd.ac.in</t>
+          <t>Williams553203@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>James Sweeney</t>
+          <t>Daniel Jones</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lewis878901@iiitd.ac.in</t>
+          <t>Charles751372@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jasmine Cameron</t>
+          <t>Daniel Rocha</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Charles19546@iiitd.ac.in</t>
+          <t>Brian403873@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jason Mcclain</t>
+          <t>Dave Reed</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mccullough991659@iiitd.ac.in</t>
+          <t>Wendy745789@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jessica Fuentes</t>
+          <t>Devin White</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nicholas589744@iiitd.ac.in</t>
+          <t>Jones543125@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jonathan Robinson</t>
+          <t>Diane Mclean</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Rogers173677@iiitd.ac.in</t>
+          <t>Norman325285@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jose Carpenter</t>
+          <t>Geoffrey Walsh</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Brennan648929@iiitd.ac.in</t>
+          <t>Logan3950@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Kathy Gonzalez</t>
+          <t>Jennifer Bowen</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ortiz183320@iiitd.ac.in</t>
+          <t>Robertson174630@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kelly Martin</t>
+          <t>Jeremy Garcia</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Debbie117627@iiitd.ac.in</t>
+          <t>Kristin253364@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Kevin Dixon</t>
+          <t>Johnathan Rios</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Gina587337@iiitd.ac.in</t>
+          <t>Perry66131@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kimberly Vasquez</t>
+          <t>Jordan Woods</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Rogers146332@iiitd.ac.in</t>
+          <t>Scott584073@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Kurt Moon</t>
+          <t>Joshua Stone</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Schwartz526904@iiitd.ac.in</t>
+          <t>Sherry623853@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Kyle Crosby</t>
+          <t>Justin Coleman</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Moore630606@iiitd.ac.in</t>
+          <t>Boyd746771@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Latoya Williams</t>
+          <t>Justin Turner</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cooper825311@iiitd.ac.in</t>
+          <t>Michael365573@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Lee Tucker</t>
+          <t>Karla Golden</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Myers345517@iiitd.ac.in</t>
+          <t>Kelly250374@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Mallory Spencer</t>
+          <t>Kevin Thompson</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Joshua649459@iiitd.ac.in</t>
+          <t>Susan252894@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mary Silva</t>
+          <t>Kim Maxwell</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Matthew60543@iiitd.ac.in</t>
+          <t>Latoya18099@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Matthew Ewing</t>
+          <t>Kirk Johnson</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ferrell216028@iiitd.ac.in</t>
+          <t>Cynthia65121@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Melissa Rice</t>
+          <t>Linda Horton</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Garcia258214@iiitd.ac.in</t>
+          <t>Harold847144@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Michael Bass</t>
+          <t>Lisa Hamilton</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Richard546738@iiitd.ac.in</t>
+          <t>Audrey206541@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Michael Fernandez</t>
+          <t>Lisa Stevens</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ashley883854@iiitd.ac.in</t>
+          <t>Andrea350343@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Michelle Yoder</t>
+          <t>Louis Phillips</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Aguilar42478@iiitd.ac.in</t>
+          <t>Kerr542453@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ms. Veronica Sanchez</t>
+          <t>Michael Coleman</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Lawrence860690@iiitd.ac.in</t>
+          <t>John575720@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Patricia Schultz</t>
+          <t>Michael Mann</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Amy745415@iiitd.ac.in</t>
+          <t>Williams311911@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Rebecca Richardson</t>
+          <t>Natalie Rhodes</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Brown150421@iiitd.ac.in</t>
+          <t>Pugh162216@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Rickey Sparks</t>
+          <t>Pamela Johnson</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Moses512656@iiitd.ac.in</t>
+          <t>Cervantes762130@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Robert Hall</t>
+          <t>Patrick Holder</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Jason162604@iiitd.ac.in</t>
+          <t>Montoya977666@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Scott Lane</t>
+          <t>Prof 2</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>King874016@iiitd.ac.in</t>
+          <t>prof2@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Stephanie Gould</t>
+          <t>Raymond Miller</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Daniel196064@iiitd.ac.in</t>
+          <t>Ricky39733@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Tammy Hamilton</t>
+          <t>Scott Henry</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Willie659819@iiitd.ac.in</t>
+          <t>Vance556791@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Tammy Ingram</t>
+          <t>Scott Smith</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Miguel129312@iiitd.ac.in</t>
+          <t>Carr651498@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Tammy Munoz</t>
+          <t>Shawn Petersen</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Eric124122@iiitd.ac.in</t>
+          <t>Clark746548@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Terrance Proctor</t>
+          <t>Sherry Walters</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Pamela740705@iiitd.ac.in</t>
+          <t>Higgins260434@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Tiffany Buck</t>
+          <t>Steven Gray</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Pamela489779@iiitd.ac.in</t>
+          <t>John394959@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Tiffany Johnson</t>
+          <t>Steven Owens</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Berger927453@iiitd.ac.in</t>
+          <t>Traci738945@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Tiffany Smith</t>
+          <t>Teresa Ramos</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ashley648062@iiitd.ac.in</t>
+          <t>Elliott473097@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Tracy Patterson</t>
+          <t>Theresa Woodward</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Justin724217@iiitd.ac.in</t>
+          <t>Scott451862@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Victor Webster</t>
+          <t>Timothy Smith</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Salazar392769@iiitd.ac.in</t>
+          <t>Edwards123676@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>William Guerrero</t>
+          <t>Zachary Hart</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Nichols15727@iiitd.ac.in</t>
+          <t>Daniel783955@iiitd.ac.in</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Zachary Estrada</t>
+          <t>prof 3</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Watson389186@iiitd.ac.in</t>
+          <t>prof3@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>William Miller</t>
+          <t>prof1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ray653580@iiitd.ac.in</t>
+          <t>prof1@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Super Advisor</t>
+          <t>prof100</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>superinstr@iiitd.ac.in</t>
+          <t>prof100@mymail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>prof7</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>prof7@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>prof8</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>prof8@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>prof9</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>prof9@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>